<commit_message>
Update hàm đọc ghi
</commit_message>
<xml_diff>
--- a/TestFile/BHBUS.xlsx
+++ b/TestFile/BHBUS.xlsx
@@ -3,12 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24102"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E906F07D-01C4-482E-94E2-D6B795514B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2171E193-0CFF-4249-9E2E-774E0CBFCAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaoHanhSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -166,18 +170,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +500,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H6" sqref="H6:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -522,12 +527,12 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
@@ -561,7 +566,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -601,14 +606,19 @@
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E6" s="6">
-        <v>44532</v>
+      <c r="D6" s="4">
+        <v>43899</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44330</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" t="str">
+        <f>IF(F6=G6,"PASS","FAIL")</f>
+        <v>FAIL</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -621,14 +631,19 @@
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E7" s="6">
-        <v>44532</v>
+      <c r="D7" s="4">
+        <v>43899</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44330</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" t="str">
+        <f t="shared" ref="H7:H11" si="0">IF(F7=G7,"PASS","FAIL")</f>
+        <v>FAIL</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -641,14 +656,19 @@
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E8" s="6">
-        <v>44532</v>
+      <c r="D8" s="4">
+        <v>43899</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44330</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -661,14 +681,19 @@
       <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E9" s="6">
-        <v>44532</v>
+      <c r="D9" s="4">
+        <v>43899</v>
+      </c>
+      <c r="E9" s="4">
+        <v>44330</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -681,14 +706,19 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E10" s="6">
-        <v>44532</v>
+      <c r="D10" s="4">
+        <v>43899</v>
+      </c>
+      <c r="E10" s="4">
+        <v>44330</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -701,14 +731,19 @@
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E11" s="6">
-        <v>44532</v>
+      <c r="D11" s="4">
+        <v>43899</v>
+      </c>
+      <c r="E11" s="4">
+        <v>44330</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
       </c>
     </row>
   </sheetData>
@@ -717,4 +752,54 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC1F49C-7BF0-4C0A-866A-4EC83FB5ACA7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B302910-C072-482A-A1A3-76DBC52EEC0C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709EBCCC-3B04-4033-8AD8-010E0549F671}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2A52C1-7909-46E5-AEFD-37288894838E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>